<commit_message>
Oct 2021 Inflation update
</commit_message>
<xml_diff>
--- a/Data/CPI and Inflation/PSA-CoreCPI.xlsx
+++ b/Data/CPI and Inflation/PSA-CoreCPI.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\RATIONALIZATION\.10_Sep2021\web\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\RATIONALIZATION\.11_Oct2021\web\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{580A7BCF-1C84-45A7-960A-4AF0B7BE5173}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E7DB183B-05BB-4D03-992D-1FDA3C13962A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1000" yWindow="250" windowWidth="17860" windowHeight="9770" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="core cpi_IR" sheetId="1" r:id="rId1"/>
@@ -89,7 +89,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="19">
   <si>
     <t>Core CPI and Core Inflation Rates in the Philippines</t>
   </si>
@@ -820,11 +820,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr syncVertical="1" syncRef="A419" transitionEvaluation="1" transitionEntry="1"/>
-  <dimension ref="A1:L441"/>
+  <dimension ref="A1:L442"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="89" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A419" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L425" sqref="L425"/>
+      <selection pane="bottomLeft" activeCell="H424" sqref="H424"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.7265625" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -8053,39 +8053,53 @@
       </c>
       <c r="I423" s="50"/>
     </row>
-    <row r="424" spans="1:9" ht="8" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A424" s="63"/>
-      <c r="B424" s="64"/>
-      <c r="C424" s="65"/>
-      <c r="D424" s="66"/>
-      <c r="E424" s="67"/>
-      <c r="F424" s="68"/>
-      <c r="G424" s="69"/>
-      <c r="H424" s="70"/>
-      <c r="I424" s="68"/>
-    </row>
-    <row r="425" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A425" s="14"/>
-      <c r="B425" s="12"/>
-      <c r="C425" s="5"/>
-      <c r="D425" s="5"/>
-      <c r="E425" s="8"/>
-      <c r="F425" s="6"/>
-      <c r="G425" s="6"/>
-      <c r="H425" s="9"/>
-      <c r="I425" s="6"/>
+    <row r="424" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A424" s="53"/>
+      <c r="B424" s="43" t="s">
+        <v>14</v>
+      </c>
+      <c r="C424" s="54"/>
+      <c r="D424" s="55"/>
+      <c r="E424" s="46">
+        <v>127.9</v>
+      </c>
+      <c r="F424" s="56"/>
+      <c r="G424" s="57"/>
+      <c r="H424" s="51">
+        <v>3.4</v>
+      </c>
+      <c r="I424" s="50"/>
+    </row>
+    <row r="425" spans="1:9" ht="17.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A425" s="63"/>
+      <c r="B425" s="64"/>
+      <c r="C425" s="65"/>
+      <c r="D425" s="66"/>
+      <c r="E425" s="67"/>
+      <c r="F425" s="68"/>
+      <c r="G425" s="69"/>
+      <c r="H425" s="70"/>
+      <c r="I425" s="68"/>
     </row>
     <row r="426" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A426" s="17" t="s">
+      <c r="A426" s="14"/>
+      <c r="B426" s="12"/>
+      <c r="C426" s="5"/>
+      <c r="D426" s="5"/>
+      <c r="E426" s="8"/>
+      <c r="F426" s="6"/>
+      <c r="G426" s="6"/>
+      <c r="H426" s="9"/>
+      <c r="I426" s="6"/>
+    </row>
+    <row r="427" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A427" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="E426" s="10"/>
-    </row>
-    <row r="427" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A427" s="15"/>
       <c r="E427" s="10"/>
     </row>
     <row r="428" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A428" s="15"/>
       <c r="E428" s="10"/>
     </row>
     <row r="429" spans="1:9" x14ac:dyDescent="0.3">
@@ -8126,6 +8140,9 @@
     </row>
     <row r="441" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E441" s="10"/>
+    </row>
+    <row r="442" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E442" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
Monthly inflation and labor update - Dec 2021
</commit_message>
<xml_diff>
--- a/Data/CPI and Inflation/PSA-CoreCPI.xlsx
+++ b/Data/CPI and Inflation/PSA-CoreCPI.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\RATIONALIZATION\.11_Oct2021\web\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\RATIONALIZATION\.11_Nov2021\web\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E7DB183B-05BB-4D03-992D-1FDA3C13962A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33F8C2CD-73FA-4088-A50F-84E1B258224A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1000" yWindow="250" windowWidth="17860" windowHeight="9770" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="core cpi_IR" sheetId="1" r:id="rId1"/>
@@ -89,7 +89,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="19">
   <si>
     <t>Core CPI and Core Inflation Rates in the Philippines</t>
   </si>
@@ -819,12 +819,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr syncVertical="1" syncRef="A419" transitionEvaluation="1" transitionEntry="1"/>
-  <dimension ref="A1:L442"/>
+  <sheetPr syncVertical="1" syncRef="A418" transitionEvaluation="1" transitionEntry="1"/>
+  <dimension ref="A1:L443"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="89" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A419" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H424" sqref="H424"/>
+      <pane ySplit="6" topLeftCell="A418" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K423" sqref="K423"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.7265625" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -8070,39 +8070,53 @@
       </c>
       <c r="I424" s="50"/>
     </row>
-    <row r="425" spans="1:9" ht="17.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A425" s="63"/>
-      <c r="B425" s="64"/>
-      <c r="C425" s="65"/>
-      <c r="D425" s="66"/>
-      <c r="E425" s="67"/>
-      <c r="F425" s="68"/>
-      <c r="G425" s="69"/>
-      <c r="H425" s="70"/>
-      <c r="I425" s="68"/>
-    </row>
-    <row r="426" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A426" s="14"/>
-      <c r="B426" s="12"/>
-      <c r="C426" s="5"/>
-      <c r="D426" s="5"/>
-      <c r="E426" s="8"/>
-      <c r="F426" s="6"/>
-      <c r="G426" s="6"/>
-      <c r="H426" s="9"/>
-      <c r="I426" s="6"/>
+    <row r="425" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A425" s="53"/>
+      <c r="B425" s="43" t="s">
+        <v>15</v>
+      </c>
+      <c r="C425" s="54"/>
+      <c r="D425" s="55"/>
+      <c r="E425" s="46">
+        <v>128.4</v>
+      </c>
+      <c r="F425" s="56"/>
+      <c r="G425" s="57"/>
+      <c r="H425" s="51">
+        <v>3.3</v>
+      </c>
+      <c r="I425" s="50"/>
+    </row>
+    <row r="426" spans="1:9" ht="17.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A426" s="63"/>
+      <c r="B426" s="64"/>
+      <c r="C426" s="65"/>
+      <c r="D426" s="66"/>
+      <c r="E426" s="67"/>
+      <c r="F426" s="68"/>
+      <c r="G426" s="69"/>
+      <c r="H426" s="70"/>
+      <c r="I426" s="68"/>
     </row>
     <row r="427" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A427" s="17" t="s">
+      <c r="A427" s="14"/>
+      <c r="B427" s="12"/>
+      <c r="C427" s="5"/>
+      <c r="D427" s="5"/>
+      <c r="E427" s="8"/>
+      <c r="F427" s="6"/>
+      <c r="G427" s="6"/>
+      <c r="H427" s="9"/>
+      <c r="I427" s="6"/>
+    </row>
+    <row r="428" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A428" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="E427" s="10"/>
-    </row>
-    <row r="428" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A428" s="15"/>
       <c r="E428" s="10"/>
     </row>
     <row r="429" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A429" s="15"/>
       <c r="E429" s="10"/>
     </row>
     <row r="430" spans="1:9" x14ac:dyDescent="0.3">
@@ -8143,6 +8157,9 @@
     </row>
     <row r="442" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E442" s="10"/>
+    </row>
+    <row r="443" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E443" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
Monthly inflation and labor update - Jan 2022
</commit_message>
<xml_diff>
--- a/Data/CPI and Inflation/PSA-CoreCPI.xlsx
+++ b/Data/CPI and Inflation/PSA-CoreCPI.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\RATIONALIZATION\.11_Nov2021\web\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\RATIONALIZATION\.12_Dec2021\web\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33F8C2CD-73FA-4088-A50F-84E1B258224A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31F84891-E4B8-4309-93C1-317C125926EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -89,7 +89,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="19">
   <si>
     <t>Core CPI and Core Inflation Rates in the Philippines</t>
   </si>
@@ -819,12 +819,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr syncVertical="1" syncRef="A418" transitionEvaluation="1" transitionEntry="1"/>
-  <dimension ref="A1:L443"/>
+  <sheetPr syncVertical="1" syncRef="A412" transitionEvaluation="1" transitionEntry="1"/>
+  <dimension ref="A1:L444"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="89" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A418" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K423" sqref="K423"/>
+      <pane ySplit="6" topLeftCell="A412" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H413" sqref="H413"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.7265625" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -7883,10 +7883,14 @@
       </c>
       <c r="C413" s="54"/>
       <c r="D413" s="55"/>
-      <c r="E413" s="46"/>
+      <c r="E413" s="46">
+        <v>126.9</v>
+      </c>
       <c r="F413" s="62"/>
       <c r="G413" s="54"/>
-      <c r="H413" s="51"/>
+      <c r="H413" s="51">
+        <v>3.3</v>
+      </c>
       <c r="I413" s="50"/>
     </row>
     <row r="414" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.4">
@@ -8087,39 +8091,53 @@
       </c>
       <c r="I425" s="50"/>
     </row>
-    <row r="426" spans="1:9" ht="17.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A426" s="63"/>
-      <c r="B426" s="64"/>
-      <c r="C426" s="65"/>
-      <c r="D426" s="66"/>
-      <c r="E426" s="67"/>
-      <c r="F426" s="68"/>
-      <c r="G426" s="69"/>
-      <c r="H426" s="70"/>
-      <c r="I426" s="68"/>
-    </row>
-    <row r="427" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A427" s="14"/>
-      <c r="B427" s="12"/>
-      <c r="C427" s="5"/>
-      <c r="D427" s="5"/>
-      <c r="E427" s="8"/>
-      <c r="F427" s="6"/>
-      <c r="G427" s="6"/>
-      <c r="H427" s="9"/>
-      <c r="I427" s="6"/>
+    <row r="426" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A426" s="53"/>
+      <c r="B426" s="43" t="s">
+        <v>16</v>
+      </c>
+      <c r="C426" s="54"/>
+      <c r="D426" s="55"/>
+      <c r="E426" s="46">
+        <v>128.6</v>
+      </c>
+      <c r="F426" s="56"/>
+      <c r="G426" s="57"/>
+      <c r="H426" s="51">
+        <v>3</v>
+      </c>
+      <c r="I426" s="50"/>
+    </row>
+    <row r="427" spans="1:9" ht="17.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A427" s="63"/>
+      <c r="B427" s="64"/>
+      <c r="C427" s="65"/>
+      <c r="D427" s="66"/>
+      <c r="E427" s="67"/>
+      <c r="F427" s="68"/>
+      <c r="G427" s="69"/>
+      <c r="H427" s="70"/>
+      <c r="I427" s="68"/>
     </row>
     <row r="428" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A428" s="17" t="s">
+      <c r="A428" s="14"/>
+      <c r="B428" s="12"/>
+      <c r="C428" s="5"/>
+      <c r="D428" s="5"/>
+      <c r="E428" s="8"/>
+      <c r="F428" s="6"/>
+      <c r="G428" s="6"/>
+      <c r="H428" s="9"/>
+      <c r="I428" s="6"/>
+    </row>
+    <row r="429" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A429" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="E428" s="10"/>
-    </row>
-    <row r="429" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A429" s="15"/>
       <c r="E429" s="10"/>
     </row>
     <row r="430" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A430" s="15"/>
       <c r="E430" s="10"/>
     </row>
     <row r="431" spans="1:9" x14ac:dyDescent="0.3">
@@ -8160,6 +8178,9 @@
     </row>
     <row r="443" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E443" s="10"/>
+    </row>
+    <row r="444" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E444" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>